<commit_message>
LISA matching steps done
</commit_message>
<xml_diff>
--- a/Public_data/Exports_CG_part1/Export_LMA_compositions.xlsx
+++ b/Public_data/Exports_CG_part1/Export_LMA_compositions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="311">
   <si>
     <t>EuralCode</t>
   </si>
@@ -229,6 +229,9 @@
     <t>electrische apparaten (vost)</t>
   </si>
   <si>
+    <t>50259</t>
+  </si>
+  <si>
     <t>elektrische apparaten [vost]</t>
   </si>
   <si>
@@ -574,9 +577,6 @@
     <t>kei</t>
   </si>
   <si>
-    <t>niet onder 20 01 21 en 20 01 23 vallende afgedankte elektrische en elektronische apparatuur die gevaarlijke onderdelen  3 bevat</t>
-  </si>
-  <si>
     <t>wit- en bruingoed, extern</t>
   </si>
   <si>
@@ -622,7 +622,7 @@
     <t>koelapparatuur (algemeen)</t>
   </si>
   <si>
-    <t>electrische componenten  &amp;amp;lt; 500 ltr</t>
+    <t>electrische componenten &amp;amp;lt; 500 ltr</t>
   </si>
   <si>
     <t>electronicaprodukten</t>
@@ -865,16 +865,13 @@
     <t>batterijen en acuu's</t>
   </si>
   <si>
-    <t>batterijen  &amp;amp;lt;  1kg/stuk</t>
-  </si>
-  <si>
-    <t>batterijen &amp;amp;lt;  1kg/stuk</t>
+    <t>batterijen &amp;amp;lt; 1kg/stuk</t>
   </si>
   <si>
     <t>batterijen &amp;amp;gt; 1 kg</t>
   </si>
   <si>
-    <t>batterijen &amp;lt;  1kg/stuk</t>
+    <t>batterijen &amp;lt; 1kg/stuk</t>
   </si>
   <si>
     <t>loodaccu&amp;amp;apos;s</t>
@@ -883,7 +880,7 @@
     <t>loodaccu&amp;apos;s</t>
   </si>
   <si>
-    <t>batterijen &amp;lt;  3kg/stuk</t>
+    <t>batterijen &amp;lt; 3kg/stuk</t>
   </si>
   <si>
     <t>batterijen &amp;lt; 3 kg/stuk</t>
@@ -904,7 +901,7 @@
     <t>batterijen lichter dan 1 kilogram</t>
   </si>
   <si>
-    <t>batterijen  &amp;amp;lt;  1kg</t>
+    <t>batterijen &amp;amp;lt; 1kg</t>
   </si>
   <si>
     <t>nikkel-cadmium accu's</t>
@@ -934,7 +931,7 @@
     <t>accus</t>
   </si>
   <si>
-    <t>batterijen (droog )  &amp;amp;lt; 1kg</t>
+    <t>batterijen (droog ) &amp;amp;lt; 1kg</t>
   </si>
   <si>
     <t>vernietiging knoopcel lithiumbatterijen</t>
@@ -1307,7 +1304,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C350"/>
+  <dimension ref="A1:C348"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2087,6 +2084,9 @@
       <c r="B71">
         <v>200136</v>
       </c>
+      <c r="C71" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1">
@@ -2096,7 +2096,7 @@
         <v>200136</v>
       </c>
       <c r="C72" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2107,7 +2107,7 @@
         <v>200136</v>
       </c>
       <c r="C73" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2118,7 +2118,7 @@
         <v>200136</v>
       </c>
       <c r="C74" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2129,7 +2129,7 @@
         <v>200136</v>
       </c>
       <c r="C75" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2140,7 +2140,7 @@
         <v>200136</v>
       </c>
       <c r="C76" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2151,7 +2151,7 @@
         <v>200136</v>
       </c>
       <c r="C77" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2162,7 +2162,7 @@
         <v>200136</v>
       </c>
       <c r="C78" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2173,7 +2173,7 @@
         <v>200136</v>
       </c>
       <c r="C79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2184,7 +2184,7 @@
         <v>200136</v>
       </c>
       <c r="C80" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2195,7 +2195,7 @@
         <v>200136</v>
       </c>
       <c r="C81" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2206,7 +2206,7 @@
         <v>200136</v>
       </c>
       <c r="C82" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2217,7 +2217,7 @@
         <v>200136</v>
       </c>
       <c r="C83" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2228,7 +2228,7 @@
         <v>200136</v>
       </c>
       <c r="C84" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2239,7 +2239,7 @@
         <v>200136</v>
       </c>
       <c r="C85" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2250,7 +2250,7 @@
         <v>200136</v>
       </c>
       <c r="C86" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2261,7 +2261,7 @@
         <v>200136</v>
       </c>
       <c r="C87" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2272,7 +2272,7 @@
         <v>200136</v>
       </c>
       <c r="C88" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2283,7 +2283,7 @@
         <v>200136</v>
       </c>
       <c r="C89" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2294,7 +2294,7 @@
         <v>200136</v>
       </c>
       <c r="C90" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2305,7 +2305,7 @@
         <v>200136</v>
       </c>
       <c r="C91" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2316,7 +2316,7 @@
         <v>200136</v>
       </c>
       <c r="C92" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2327,7 +2327,7 @@
         <v>200136</v>
       </c>
       <c r="C93" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2338,7 +2338,7 @@
         <v>200136</v>
       </c>
       <c r="C94" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2349,7 +2349,7 @@
         <v>200136</v>
       </c>
       <c r="C95" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2360,7 +2360,7 @@
         <v>200136</v>
       </c>
       <c r="C96" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2371,7 +2371,7 @@
         <v>200136</v>
       </c>
       <c r="C97" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2382,7 +2382,7 @@
         <v>200136</v>
       </c>
       <c r="C98" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2393,7 +2393,7 @@
         <v>200136</v>
       </c>
       <c r="C99" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2404,7 +2404,7 @@
         <v>200136</v>
       </c>
       <c r="C100" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2415,7 +2415,7 @@
         <v>200136</v>
       </c>
       <c r="C101" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2426,7 +2426,7 @@
         <v>200136</v>
       </c>
       <c r="C102" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2437,7 +2437,7 @@
         <v>200136</v>
       </c>
       <c r="C103" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2448,7 +2448,7 @@
         <v>200136</v>
       </c>
       <c r="C104" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2459,7 +2459,7 @@
         <v>200136</v>
       </c>
       <c r="C105" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2470,7 +2470,7 @@
         <v>200136</v>
       </c>
       <c r="C106" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2481,7 +2481,7 @@
         <v>200136</v>
       </c>
       <c r="C107" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2492,7 +2492,7 @@
         <v>200136</v>
       </c>
       <c r="C108" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2503,7 +2503,7 @@
         <v>200136</v>
       </c>
       <c r="C109" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2514,7 +2514,7 @@
         <v>200136</v>
       </c>
       <c r="C110" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2525,7 +2525,7 @@
         <v>200136</v>
       </c>
       <c r="C111" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2536,7 +2536,7 @@
         <v>200136</v>
       </c>
       <c r="C112" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2547,7 +2547,7 @@
         <v>200136</v>
       </c>
       <c r="C113" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2558,7 +2558,7 @@
         <v>200136</v>
       </c>
       <c r="C114" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2569,7 +2569,7 @@
         <v>200136</v>
       </c>
       <c r="C115" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2580,7 +2580,7 @@
         <v>200136</v>
       </c>
       <c r="C116" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2591,7 +2591,7 @@
         <v>200136</v>
       </c>
       <c r="C117" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2602,7 +2602,7 @@
         <v>200136</v>
       </c>
       <c r="C118" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2613,7 +2613,7 @@
         <v>200136</v>
       </c>
       <c r="C119" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2624,7 +2624,7 @@
         <v>200136</v>
       </c>
       <c r="C120" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2635,7 +2635,7 @@
         <v>200136</v>
       </c>
       <c r="C121" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2646,7 +2646,7 @@
         <v>200136</v>
       </c>
       <c r="C122" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2657,7 +2657,7 @@
         <v>200136</v>
       </c>
       <c r="C123" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2668,7 +2668,7 @@
         <v>200136</v>
       </c>
       <c r="C124" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2679,7 +2679,7 @@
         <v>200136</v>
       </c>
       <c r="C125" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2690,7 +2690,7 @@
         <v>200136</v>
       </c>
       <c r="C126" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2701,7 +2701,7 @@
         <v>200136</v>
       </c>
       <c r="C127" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2712,7 +2712,7 @@
         <v>200136</v>
       </c>
       <c r="C128" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2723,7 +2723,7 @@
         <v>200136</v>
       </c>
       <c r="C129" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2734,7 +2734,7 @@
         <v>200136</v>
       </c>
       <c r="C130" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2745,7 +2745,7 @@
         <v>200136</v>
       </c>
       <c r="C131" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2756,7 +2756,7 @@
         <v>200136</v>
       </c>
       <c r="C132" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2767,7 +2767,7 @@
         <v>200136</v>
       </c>
       <c r="C133" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2778,7 +2778,7 @@
         <v>200136</v>
       </c>
       <c r="C134" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2789,7 +2789,7 @@
         <v>200136</v>
       </c>
       <c r="C135" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2800,7 +2800,7 @@
         <v>200136</v>
       </c>
       <c r="C136" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2811,7 +2811,7 @@
         <v>200136</v>
       </c>
       <c r="C137" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2822,7 +2822,7 @@
         <v>200136</v>
       </c>
       <c r="C138" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2833,7 +2833,7 @@
         <v>200136</v>
       </c>
       <c r="C139" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2844,7 +2844,7 @@
         <v>200136</v>
       </c>
       <c r="C140" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2855,7 +2855,7 @@
         <v>200136</v>
       </c>
       <c r="C141" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2866,7 +2866,7 @@
         <v>200136</v>
       </c>
       <c r="C142" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2877,7 +2877,7 @@
         <v>200136</v>
       </c>
       <c r="C143" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2888,7 +2888,7 @@
         <v>200136</v>
       </c>
       <c r="C144" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2899,7 +2899,7 @@
         <v>200136</v>
       </c>
       <c r="C145" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2910,7 +2910,7 @@
         <v>200136</v>
       </c>
       <c r="C146" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2921,7 +2921,7 @@
         <v>200136</v>
       </c>
       <c r="C147" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2932,7 +2932,7 @@
         <v>200136</v>
       </c>
       <c r="C148" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2943,7 +2943,7 @@
         <v>200136</v>
       </c>
       <c r="C149" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2954,7 +2954,7 @@
         <v>200136</v>
       </c>
       <c r="C150" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2965,7 +2965,7 @@
         <v>200136</v>
       </c>
       <c r="C151" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2976,7 +2976,7 @@
         <v>200136</v>
       </c>
       <c r="C152" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2987,7 +2987,7 @@
         <v>200136</v>
       </c>
       <c r="C153" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2998,7 +2998,7 @@
         <v>200136</v>
       </c>
       <c r="C154" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -3009,7 +3009,7 @@
         <v>200136</v>
       </c>
       <c r="C155" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -3020,7 +3020,7 @@
         <v>200136</v>
       </c>
       <c r="C156" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -3031,7 +3031,7 @@
         <v>200136</v>
       </c>
       <c r="C157" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3042,7 +3042,7 @@
         <v>200136</v>
       </c>
       <c r="C158" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -3053,7 +3053,7 @@
         <v>200136</v>
       </c>
       <c r="C159" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3064,7 +3064,7 @@
         <v>200136</v>
       </c>
       <c r="C160" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3075,7 +3075,7 @@
         <v>200136</v>
       </c>
       <c r="C161" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -3086,7 +3086,7 @@
         <v>200136</v>
       </c>
       <c r="C162" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3097,7 +3097,7 @@
         <v>200136</v>
       </c>
       <c r="C163" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3108,7 +3108,7 @@
         <v>200136</v>
       </c>
       <c r="C164" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3119,7 +3119,7 @@
         <v>200136</v>
       </c>
       <c r="C165" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3130,7 +3130,7 @@
         <v>200136</v>
       </c>
       <c r="C166" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3141,7 +3141,7 @@
         <v>200136</v>
       </c>
       <c r="C167" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3152,7 +3152,7 @@
         <v>200136</v>
       </c>
       <c r="C168" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3163,7 +3163,7 @@
         <v>200136</v>
       </c>
       <c r="C169" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3174,7 +3174,7 @@
         <v>200135</v>
       </c>
       <c r="C170" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3196,7 +3196,7 @@
         <v>200135</v>
       </c>
       <c r="C172" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3207,7 +3207,7 @@
         <v>200135</v>
       </c>
       <c r="C173" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3218,7 +3218,7 @@
         <v>200135</v>
       </c>
       <c r="C174" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3229,7 +3229,7 @@
         <v>200135</v>
       </c>
       <c r="C175" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3240,7 +3240,7 @@
         <v>200135</v>
       </c>
       <c r="C176" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3251,7 +3251,7 @@
         <v>200135</v>
       </c>
       <c r="C177" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3273,7 +3273,7 @@
         <v>200135</v>
       </c>
       <c r="C179" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3284,7 +3284,7 @@
         <v>200135</v>
       </c>
       <c r="C180" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3295,7 +3295,7 @@
         <v>200135</v>
       </c>
       <c r="C181" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3306,7 +3306,7 @@
         <v>200135</v>
       </c>
       <c r="C182" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3317,7 +3317,7 @@
         <v>200135</v>
       </c>
       <c r="C183" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3328,7 +3328,7 @@
         <v>200135</v>
       </c>
       <c r="C184" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3339,7 +3339,7 @@
         <v>200135</v>
       </c>
       <c r="C185" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3350,7 +3350,7 @@
         <v>200135</v>
       </c>
       <c r="C186" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3361,7 +3361,7 @@
         <v>200135</v>
       </c>
       <c r="C187" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3372,7 +3372,7 @@
         <v>200135</v>
       </c>
       <c r="C188" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3383,1090 +3383,1090 @@
         <v>200135</v>
       </c>
       <c r="C189" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="1">
-        <v>2572</v>
+        <v>2616</v>
       </c>
       <c r="B190">
         <v>200135</v>
       </c>
       <c r="C190" t="s">
-        <v>186</v>
+        <v>62</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="1">
-        <v>2616</v>
+        <v>2704</v>
       </c>
       <c r="B191">
         <v>200135</v>
       </c>
       <c r="C191" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="1">
-        <v>2704</v>
+        <v>2708</v>
       </c>
       <c r="B192">
         <v>200135</v>
       </c>
       <c r="C192" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="1">
-        <v>2708</v>
+        <v>2713</v>
       </c>
       <c r="B193">
         <v>200135</v>
       </c>
       <c r="C193" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="1">
-        <v>2713</v>
+        <v>2722</v>
       </c>
       <c r="B194">
         <v>200135</v>
       </c>
       <c r="C194" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="1">
-        <v>2722</v>
+        <v>2741</v>
       </c>
       <c r="B195">
         <v>200135</v>
       </c>
       <c r="C195" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="1">
-        <v>2741</v>
+        <v>2768</v>
       </c>
       <c r="B196">
         <v>200135</v>
       </c>
       <c r="C196" t="s">
-        <v>51</v>
+        <v>187</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="1">
-        <v>2768</v>
+        <v>2787</v>
       </c>
       <c r="B197">
         <v>200135</v>
       </c>
       <c r="C197" t="s">
-        <v>187</v>
+        <v>37</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="1">
-        <v>2787</v>
+        <v>2829</v>
       </c>
       <c r="B198">
         <v>200135</v>
       </c>
       <c r="C198" t="s">
-        <v>37</v>
+        <v>188</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="1">
-        <v>2829</v>
+        <v>2835</v>
       </c>
       <c r="B199">
         <v>200135</v>
       </c>
       <c r="C199" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="1">
-        <v>2835</v>
+        <v>2838</v>
       </c>
       <c r="B200">
         <v>200135</v>
       </c>
       <c r="C200" t="s">
-        <v>189</v>
+        <v>83</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="1">
-        <v>2838</v>
+        <v>2851</v>
       </c>
       <c r="B201">
         <v>200135</v>
       </c>
       <c r="C201" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="1">
-        <v>2851</v>
+        <v>2870</v>
       </c>
       <c r="B202">
         <v>200135</v>
       </c>
       <c r="C202" t="s">
-        <v>90</v>
+        <v>190</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="1">
-        <v>2870</v>
+        <v>2896</v>
       </c>
       <c r="B203">
         <v>200135</v>
       </c>
       <c r="C203" t="s">
-        <v>190</v>
+        <v>86</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="1">
-        <v>2896</v>
+        <v>2916</v>
       </c>
       <c r="B204">
         <v>200135</v>
       </c>
       <c r="C204" t="s">
-        <v>85</v>
+        <v>191</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="1">
-        <v>2916</v>
+        <v>2944</v>
       </c>
       <c r="B205">
         <v>200135</v>
       </c>
       <c r="C205" t="s">
-        <v>191</v>
+        <v>34</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="1">
-        <v>2944</v>
+        <v>2946</v>
       </c>
       <c r="B206">
         <v>200135</v>
       </c>
       <c r="C206" t="s">
-        <v>34</v>
+        <v>192</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="1">
-        <v>2946</v>
+        <v>2947</v>
       </c>
       <c r="B207">
         <v>200135</v>
       </c>
       <c r="C207" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="1">
-        <v>2947</v>
+        <v>2954</v>
       </c>
       <c r="B208">
         <v>200135</v>
       </c>
       <c r="C208" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="1">
-        <v>2954</v>
+        <v>2955</v>
       </c>
       <c r="B209">
         <v>200135</v>
       </c>
       <c r="C209" t="s">
-        <v>194</v>
+        <v>60</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="1">
-        <v>2955</v>
+        <v>2969</v>
       </c>
       <c r="B210">
         <v>200135</v>
       </c>
       <c r="C210" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="1">
-        <v>2969</v>
+        <v>2974</v>
       </c>
       <c r="B211">
         <v>200135</v>
       </c>
       <c r="C211" t="s">
-        <v>49</v>
+        <v>195</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="1">
-        <v>2974</v>
+        <v>2975</v>
       </c>
       <c r="B212">
         <v>200135</v>
       </c>
       <c r="C212" t="s">
-        <v>195</v>
+        <v>97</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="1">
-        <v>2975</v>
+        <v>2995</v>
       </c>
       <c r="B213">
         <v>200135</v>
       </c>
       <c r="C213" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="1">
-        <v>2995</v>
+        <v>2996</v>
       </c>
       <c r="B214">
         <v>200135</v>
       </c>
       <c r="C214" t="s">
-        <v>50</v>
+        <v>196</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="1">
-        <v>2996</v>
+        <v>3024</v>
       </c>
       <c r="B215">
         <v>200135</v>
       </c>
       <c r="C215" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="1">
-        <v>3024</v>
+        <v>3026</v>
       </c>
       <c r="B216">
         <v>200135</v>
       </c>
       <c r="C216" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="1">
-        <v>3026</v>
+        <v>3034</v>
       </c>
       <c r="B217">
         <v>200135</v>
       </c>
       <c r="C217" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="1">
-        <v>3034</v>
+        <v>3053</v>
       </c>
       <c r="B218">
         <v>200135</v>
       </c>
       <c r="C218" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="1">
-        <v>3053</v>
+        <v>3070</v>
       </c>
       <c r="B219">
         <v>200135</v>
       </c>
       <c r="C219" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="1">
-        <v>3070</v>
+        <v>3076</v>
       </c>
       <c r="B220">
         <v>200135</v>
       </c>
       <c r="C220" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="1">
-        <v>3076</v>
+        <v>3088</v>
       </c>
       <c r="B221">
         <v>200135</v>
       </c>
       <c r="C221" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="1">
-        <v>3088</v>
+        <v>3091</v>
       </c>
       <c r="B222">
         <v>200135</v>
       </c>
       <c r="C222" t="s">
-        <v>103</v>
+        <v>203</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="1">
-        <v>3091</v>
+        <v>3096</v>
       </c>
       <c r="B223">
         <v>200135</v>
       </c>
       <c r="C223" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="1">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="B224">
         <v>200135</v>
       </c>
       <c r="C224" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="1">
-        <v>3097</v>
+        <v>3115</v>
       </c>
       <c r="B225">
         <v>200135</v>
       </c>
       <c r="C225" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="1">
-        <v>3115</v>
+        <v>3118</v>
       </c>
       <c r="B226">
         <v>200135</v>
       </c>
       <c r="C226" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="1">
-        <v>3118</v>
+        <v>3130</v>
       </c>
       <c r="B227">
         <v>200135</v>
       </c>
       <c r="C227" t="s">
-        <v>167</v>
+        <v>207</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="1">
-        <v>3130</v>
+        <v>3135</v>
       </c>
       <c r="B228">
         <v>200135</v>
       </c>
       <c r="C228" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" s="1">
-        <v>3135</v>
+        <v>3163</v>
       </c>
       <c r="B229">
         <v>200135</v>
       </c>
       <c r="C229" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="1">
-        <v>3163</v>
+        <v>3206</v>
       </c>
       <c r="B230">
         <v>200135</v>
       </c>
       <c r="C230" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="1">
-        <v>3206</v>
+        <v>3219</v>
       </c>
       <c r="B231">
         <v>200135</v>
       </c>
       <c r="C231" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="1">
-        <v>3219</v>
+        <v>3235</v>
       </c>
       <c r="B232">
         <v>200135</v>
       </c>
       <c r="C232" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="1">
-        <v>3235</v>
+        <v>3302</v>
       </c>
       <c r="B233">
         <v>200135</v>
       </c>
       <c r="C233" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="1">
-        <v>3302</v>
+        <v>3313</v>
       </c>
       <c r="B234">
         <v>200135</v>
       </c>
       <c r="C234" t="s">
-        <v>213</v>
+        <v>115</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="1">
-        <v>3313</v>
+        <v>3314</v>
       </c>
       <c r="B235">
         <v>200135</v>
       </c>
       <c r="C235" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="1">
-        <v>3314</v>
+        <v>3328</v>
       </c>
       <c r="B236">
         <v>200135</v>
       </c>
       <c r="C236" t="s">
-        <v>75</v>
+        <v>214</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="1">
-        <v>3328</v>
+        <v>3355</v>
       </c>
       <c r="B237">
         <v>200135</v>
       </c>
       <c r="C237" t="s">
-        <v>214</v>
+        <v>122</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="1">
-        <v>3355</v>
+        <v>3403</v>
       </c>
       <c r="B238">
         <v>200135</v>
       </c>
       <c r="C238" t="s">
-        <v>121</v>
+        <v>215</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="1">
-        <v>3403</v>
+        <v>3405</v>
       </c>
       <c r="B239">
         <v>200135</v>
       </c>
       <c r="C239" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" s="1">
-        <v>3405</v>
+        <v>3409</v>
       </c>
       <c r="B240">
         <v>200135</v>
       </c>
       <c r="C240" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="1">
-        <v>3409</v>
+        <v>3410</v>
       </c>
       <c r="B241">
         <v>200135</v>
       </c>
       <c r="C241" t="s">
-        <v>217</v>
+        <v>58</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="1">
-        <v>3410</v>
+        <v>3411</v>
       </c>
       <c r="B242">
         <v>200135</v>
       </c>
       <c r="C242" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="1">
-        <v>3411</v>
+        <v>3414</v>
       </c>
       <c r="B243">
         <v>200135</v>
       </c>
       <c r="C243" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="1">
-        <v>3414</v>
+        <v>3417</v>
       </c>
       <c r="B244">
         <v>200135</v>
       </c>
       <c r="C244" t="s">
-        <v>154</v>
+        <v>218</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="1">
-        <v>3417</v>
+        <v>3419</v>
       </c>
       <c r="B245">
         <v>200135</v>
       </c>
       <c r="C245" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="1">
-        <v>3419</v>
+        <v>3422</v>
       </c>
       <c r="B246">
         <v>200135</v>
       </c>
       <c r="C246" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="1">
-        <v>3422</v>
+        <v>3433</v>
       </c>
       <c r="B247">
         <v>200135</v>
       </c>
       <c r="C247" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="1">
-        <v>3433</v>
+        <v>3444</v>
       </c>
       <c r="B248">
         <v>200135</v>
       </c>
       <c r="C248" t="s">
-        <v>221</v>
+        <v>156</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="1">
-        <v>3444</v>
+        <v>3476</v>
       </c>
       <c r="B249">
         <v>200135</v>
       </c>
       <c r="C249" t="s">
-        <v>155</v>
+        <v>222</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" s="1">
-        <v>3476</v>
+        <v>3481</v>
       </c>
       <c r="B250">
         <v>200135</v>
       </c>
       <c r="C250" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="1">
-        <v>3481</v>
+        <v>3490</v>
       </c>
       <c r="B251">
         <v>200135</v>
       </c>
       <c r="C251" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="1">
-        <v>3490</v>
+        <v>3491</v>
       </c>
       <c r="B252">
         <v>200135</v>
       </c>
       <c r="C252" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" s="1">
-        <v>3491</v>
+        <v>3492</v>
       </c>
       <c r="B253">
         <v>200135</v>
       </c>
       <c r="C253" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" s="1">
-        <v>3492</v>
+        <v>3502</v>
       </c>
       <c r="B254">
         <v>200135</v>
       </c>
       <c r="C254" t="s">
-        <v>226</v>
+        <v>113</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" s="1">
-        <v>3502</v>
+        <v>3503</v>
       </c>
       <c r="B255">
         <v>200135</v>
       </c>
       <c r="C255" t="s">
-        <v>112</v>
+        <v>227</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="1">
-        <v>3503</v>
+        <v>3505</v>
       </c>
       <c r="B256">
         <v>200135</v>
       </c>
       <c r="C256" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="1">
-        <v>3505</v>
+        <v>3506</v>
       </c>
       <c r="B257">
         <v>200135</v>
       </c>
       <c r="C257" t="s">
-        <v>228</v>
+        <v>36</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="1">
-        <v>3506</v>
+        <v>3524</v>
       </c>
       <c r="B258">
         <v>200135</v>
       </c>
       <c r="C258" t="s">
-        <v>36</v>
+        <v>229</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="1">
-        <v>3524</v>
+        <v>3525</v>
       </c>
       <c r="B259">
         <v>200135</v>
       </c>
       <c r="C259" t="s">
-        <v>229</v>
+        <v>126</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="1">
-        <v>3525</v>
+        <v>3546</v>
       </c>
       <c r="B260">
         <v>200135</v>
       </c>
       <c r="C260" t="s">
-        <v>125</v>
+        <v>230</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="1">
-        <v>3546</v>
+        <v>3553</v>
       </c>
       <c r="B261">
         <v>200135</v>
       </c>
       <c r="C261" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="1">
-        <v>3553</v>
+        <v>3585</v>
       </c>
       <c r="B262">
         <v>200135</v>
       </c>
       <c r="C262" t="s">
-        <v>231</v>
+        <v>63</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" s="1">
-        <v>3585</v>
+        <v>3679</v>
       </c>
       <c r="B263">
         <v>200135</v>
       </c>
       <c r="C263" t="s">
-        <v>63</v>
+        <v>139</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="1">
-        <v>3679</v>
+        <v>3692</v>
       </c>
       <c r="B264">
         <v>200135</v>
       </c>
       <c r="C264" t="s">
-        <v>138</v>
+        <v>232</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" s="1">
-        <v>3692</v>
+        <v>3696</v>
       </c>
       <c r="B265">
         <v>200135</v>
       </c>
       <c r="C265" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" s="1">
-        <v>3696</v>
+        <v>3700</v>
       </c>
       <c r="B266">
         <v>200135</v>
       </c>
       <c r="C266" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" s="1">
-        <v>3700</v>
+        <v>3701</v>
       </c>
       <c r="B267">
         <v>200135</v>
       </c>
       <c r="C267" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" s="1">
-        <v>3701</v>
+        <v>3741</v>
       </c>
       <c r="B268">
         <v>200135</v>
       </c>
       <c r="C268" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="1">
-        <v>3741</v>
+        <v>3744</v>
       </c>
       <c r="B269">
         <v>200135</v>
       </c>
       <c r="C269" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" s="1">
-        <v>3744</v>
+        <v>3752</v>
       </c>
       <c r="B270">
         <v>200135</v>
       </c>
       <c r="C270" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="1">
-        <v>3752</v>
+        <v>3753</v>
       </c>
       <c r="B271">
         <v>200135</v>
       </c>
       <c r="C271" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="1">
-        <v>3753</v>
+        <v>3755</v>
       </c>
       <c r="B272">
         <v>200135</v>
       </c>
       <c r="C272" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" s="1">
-        <v>3755</v>
+        <v>3756</v>
       </c>
       <c r="B273">
         <v>200135</v>
       </c>
       <c r="C273" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" s="1">
-        <v>3756</v>
+        <v>3762</v>
       </c>
       <c r="B274">
         <v>200135</v>
       </c>
       <c r="C274" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="275" spans="1:3">
       <c r="A275" s="1">
-        <v>3762</v>
+        <v>3765</v>
       </c>
       <c r="B275">
         <v>200135</v>
       </c>
       <c r="C275" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" s="1">
-        <v>3765</v>
+        <v>3768</v>
       </c>
       <c r="B276">
         <v>200135</v>
       </c>
       <c r="C276" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" s="1">
-        <v>3768</v>
+        <v>3775</v>
       </c>
       <c r="B277">
         <v>200135</v>
       </c>
       <c r="C277" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" s="1">
-        <v>3775</v>
+        <v>3776</v>
       </c>
       <c r="B278">
         <v>200135</v>
       </c>
       <c r="C278" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="1">
-        <v>3776</v>
+        <v>3778</v>
       </c>
       <c r="B279">
         <v>200135</v>
       </c>
       <c r="C279" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="1">
-        <v>3778</v>
+        <v>3784</v>
       </c>
       <c r="B280">
         <v>200135</v>
       </c>
       <c r="C280" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="1">
-        <v>3784</v>
+        <v>3943</v>
       </c>
       <c r="B281">
         <v>200135</v>
       </c>
       <c r="C281" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="1">
-        <v>3943</v>
+        <v>3957</v>
       </c>
       <c r="B282">
         <v>200135</v>
       </c>
       <c r="C282" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="1">
-        <v>3957</v>
+        <v>3966</v>
       </c>
       <c r="B283">
         <v>200135</v>
       </c>
       <c r="C283" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="1">
-        <v>3966</v>
+        <v>3967</v>
       </c>
       <c r="B284">
         <v>200135</v>
       </c>
       <c r="C284" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="1">
-        <v>3967</v>
+        <v>3969</v>
       </c>
       <c r="B285">
         <v>200135</v>
       </c>
       <c r="C285" t="s">
-        <v>252</v>
+        <v>46</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" s="1">
-        <v>3969</v>
+        <v>3978</v>
       </c>
       <c r="B286">
         <v>200135</v>
       </c>
       <c r="C286" t="s">
-        <v>46</v>
+        <v>253</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" s="1">
-        <v>3978</v>
+        <v>3989</v>
       </c>
       <c r="B287">
         <v>200135</v>
       </c>
       <c r="C287" t="s">
-        <v>253</v>
+        <v>129</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" s="1">
-        <v>3989</v>
+        <v>3999</v>
       </c>
       <c r="B288">
         <v>200135</v>
@@ -4477,684 +4477,662 @@
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="1">
-        <v>3999</v>
+        <v>4002</v>
       </c>
       <c r="B289">
         <v>200135</v>
       </c>
       <c r="C289" t="s">
-        <v>127</v>
+        <v>254</v>
       </c>
     </row>
     <row r="290" spans="1:3">
       <c r="A290" s="1">
-        <v>4002</v>
+        <v>4026</v>
       </c>
       <c r="B290">
         <v>200135</v>
       </c>
       <c r="C290" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="1">
-        <v>4026</v>
+        <v>4067</v>
       </c>
       <c r="B291">
         <v>200135</v>
       </c>
       <c r="C291" t="s">
-        <v>255</v>
+        <v>161</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" s="1">
-        <v>4067</v>
+        <v>4068</v>
       </c>
       <c r="B292">
         <v>200135</v>
       </c>
       <c r="C292" t="s">
-        <v>160</v>
+        <v>256</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" s="1">
-        <v>4068</v>
+        <v>4079</v>
       </c>
       <c r="B293">
         <v>200135</v>
       </c>
       <c r="C293" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="1">
-        <v>4079</v>
+        <v>4149</v>
       </c>
       <c r="B294">
         <v>200135</v>
       </c>
       <c r="C294" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="A295" s="1">
-        <v>4149</v>
+        <v>4316</v>
       </c>
       <c r="B295">
         <v>200135</v>
       </c>
       <c r="C295" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" s="1">
-        <v>4316</v>
+        <v>4319</v>
       </c>
       <c r="B296">
         <v>200135</v>
       </c>
       <c r="C296" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" s="1">
-        <v>4319</v>
+        <v>4334</v>
       </c>
       <c r="B297">
         <v>200135</v>
       </c>
       <c r="C297" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="1">
-        <v>4334</v>
+        <v>4335</v>
       </c>
       <c r="B298">
-        <v>200135</v>
+        <v>200133</v>
       </c>
       <c r="C298" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="299" spans="1:3">
       <c r="A299" s="1">
-        <v>4335</v>
+        <v>4341</v>
       </c>
       <c r="B299">
         <v>200133</v>
       </c>
       <c r="C299" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="300" spans="1:3">
       <c r="A300" s="1">
-        <v>4341</v>
+        <v>4345</v>
       </c>
       <c r="B300">
         <v>200133</v>
       </c>
       <c r="C300" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="301" spans="1:3">
       <c r="A301" s="1">
-        <v>4345</v>
+        <v>4346</v>
       </c>
       <c r="B301">
         <v>200133</v>
       </c>
       <c r="C301" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="1">
-        <v>4346</v>
+        <v>4347</v>
       </c>
       <c r="B302">
         <v>200133</v>
       </c>
       <c r="C302" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="303" spans="1:3">
       <c r="A303" s="1">
-        <v>4347</v>
+        <v>4348</v>
       </c>
       <c r="B303">
         <v>200133</v>
       </c>
       <c r="C303" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="304" spans="1:3">
       <c r="A304" s="1">
-        <v>4348</v>
+        <v>4453</v>
       </c>
       <c r="B304">
         <v>200133</v>
       </c>
       <c r="C304" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="A305" s="1">
-        <v>4453</v>
+        <v>4510</v>
       </c>
       <c r="B305">
         <v>200133</v>
       </c>
       <c r="C305" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="306" spans="1:3">
       <c r="A306" s="1">
-        <v>4510</v>
+        <v>4636</v>
       </c>
       <c r="B306">
         <v>200133</v>
       </c>
       <c r="C306" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="307" spans="1:3">
       <c r="A307" s="1">
-        <v>4636</v>
+        <v>4665</v>
       </c>
       <c r="B307">
         <v>200133</v>
       </c>
       <c r="C307" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="308" spans="1:3">
       <c r="A308" s="1">
-        <v>4665</v>
+        <v>4776</v>
       </c>
       <c r="B308">
         <v>200133</v>
       </c>
       <c r="C308" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="309" spans="1:3">
       <c r="A309" s="1">
-        <v>4776</v>
+        <v>5010</v>
       </c>
       <c r="B309">
         <v>200133</v>
       </c>
       <c r="C309" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="310" spans="1:3">
       <c r="A310" s="1">
-        <v>5010</v>
+        <v>5154</v>
       </c>
       <c r="B310">
         <v>200133</v>
       </c>
       <c r="C310" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="311" spans="1:3">
       <c r="A311" s="1">
-        <v>5154</v>
+        <v>5563</v>
       </c>
       <c r="B311">
         <v>200133</v>
       </c>
       <c r="C311" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="312" spans="1:3">
       <c r="A312" s="1">
-        <v>5563</v>
+        <v>5569</v>
       </c>
       <c r="B312">
         <v>200133</v>
       </c>
       <c r="C312" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="1">
-        <v>5569</v>
+        <v>5584</v>
       </c>
       <c r="B313">
         <v>200133</v>
       </c>
       <c r="C313" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="314" spans="1:3">
       <c r="A314" s="1">
-        <v>5584</v>
+        <v>5600</v>
       </c>
       <c r="B314">
         <v>200133</v>
       </c>
       <c r="C314" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="315" spans="1:3">
       <c r="A315" s="1">
-        <v>5600</v>
+        <v>5614</v>
       </c>
       <c r="B315">
         <v>200133</v>
       </c>
       <c r="C315" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="316" spans="1:3">
       <c r="A316" s="1">
-        <v>5614</v>
+        <v>5621</v>
       </c>
       <c r="B316">
         <v>200133</v>
       </c>
       <c r="C316" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="317" spans="1:3">
       <c r="A317" s="1">
-        <v>5621</v>
+        <v>5622</v>
       </c>
       <c r="B317">
         <v>200133</v>
       </c>
       <c r="C317" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="318" spans="1:3">
       <c r="A318" s="1">
-        <v>5622</v>
+        <v>5650</v>
       </c>
       <c r="B318">
         <v>200133</v>
       </c>
       <c r="C318" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="319" spans="1:3">
       <c r="A319" s="1">
-        <v>5650</v>
+        <v>5704</v>
       </c>
       <c r="B319">
         <v>200133</v>
       </c>
       <c r="C319" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="1">
-        <v>5704</v>
+        <v>5741</v>
       </c>
       <c r="B320">
         <v>200133</v>
       </c>
       <c r="C320" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="1">
-        <v>5708</v>
+        <v>5787</v>
       </c>
       <c r="B321">
         <v>200133</v>
       </c>
       <c r="C321" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322" s="1">
-        <v>5741</v>
+        <v>5825</v>
       </c>
       <c r="B322">
         <v>200133</v>
       </c>
       <c r="C322" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="323" spans="1:3">
       <c r="A323" s="1">
-        <v>5787</v>
+        <v>5931</v>
       </c>
       <c r="B323">
         <v>200133</v>
       </c>
       <c r="C323" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="324" spans="1:3">
       <c r="A324" s="1">
-        <v>5825</v>
+        <v>5942</v>
       </c>
       <c r="B324">
         <v>200133</v>
       </c>
       <c r="C324" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="325" spans="1:3">
       <c r="A325" s="1">
-        <v>5931</v>
+        <v>5944</v>
       </c>
       <c r="B325">
         <v>200133</v>
       </c>
       <c r="C325" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="326" spans="1:3">
       <c r="A326" s="1">
-        <v>5942</v>
+        <v>5980</v>
       </c>
       <c r="B326">
         <v>200133</v>
       </c>
       <c r="C326" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="327" spans="1:3">
       <c r="A327" s="1">
-        <v>5944</v>
+        <v>5999</v>
       </c>
       <c r="B327">
         <v>200133</v>
       </c>
       <c r="C327" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="328" spans="1:3">
       <c r="A328" s="1">
-        <v>5980</v>
+        <v>6027</v>
       </c>
       <c r="B328">
         <v>200133</v>
       </c>
       <c r="C328" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="329" spans="1:3">
       <c r="A329" s="1">
-        <v>5999</v>
+        <v>6029</v>
       </c>
       <c r="B329">
         <v>200133</v>
       </c>
       <c r="C329" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="330" spans="1:3">
       <c r="A330" s="1">
-        <v>6027</v>
+        <v>6048</v>
       </c>
       <c r="B330">
         <v>200133</v>
       </c>
       <c r="C330" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="331" spans="1:3">
       <c r="A331" s="1">
-        <v>6029</v>
+        <v>6054</v>
       </c>
       <c r="B331">
         <v>200133</v>
       </c>
       <c r="C331" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="332" spans="1:3">
       <c r="A332" s="1">
-        <v>6048</v>
+        <v>6098</v>
       </c>
       <c r="B332">
         <v>200133</v>
       </c>
       <c r="C332" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="333" spans="1:3">
       <c r="A333" s="1">
-        <v>6054</v>
+        <v>6145</v>
       </c>
       <c r="B333">
         <v>200133</v>
       </c>
       <c r="C333" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="334" spans="1:3">
       <c r="A334" s="1">
-        <v>6098</v>
+        <v>6146</v>
       </c>
       <c r="B334">
         <v>200133</v>
       </c>
       <c r="C334" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="335" spans="1:3">
       <c r="A335" s="1">
-        <v>6145</v>
+        <v>6262</v>
       </c>
       <c r="B335">
         <v>200133</v>
       </c>
       <c r="C335" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="336" spans="1:3">
       <c r="A336" s="1">
-        <v>6146</v>
+        <v>6353</v>
       </c>
       <c r="B336">
         <v>200133</v>
       </c>
       <c r="C336" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="337" spans="1:3">
       <c r="A337" s="1">
-        <v>6262</v>
+        <v>6570</v>
       </c>
       <c r="B337">
         <v>200133</v>
       </c>
       <c r="C337" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="338" spans="1:3">
       <c r="A338" s="1">
-        <v>6353</v>
+        <v>6601</v>
       </c>
       <c r="B338">
         <v>200133</v>
       </c>
       <c r="C338" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="339" spans="1:3">
       <c r="A339" s="1">
-        <v>6570</v>
+        <v>6630</v>
       </c>
       <c r="B339">
         <v>200133</v>
       </c>
       <c r="C339" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="340" spans="1:3">
       <c r="A340" s="1">
-        <v>6601</v>
+        <v>6637</v>
       </c>
       <c r="B340">
         <v>200133</v>
       </c>
       <c r="C340" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="341" spans="1:3">
       <c r="A341" s="1">
-        <v>6630</v>
+        <v>6699</v>
       </c>
       <c r="B341">
         <v>200133</v>
       </c>
       <c r="C341" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="342" spans="1:3">
       <c r="A342" s="1">
-        <v>6637</v>
+        <v>6938</v>
       </c>
       <c r="B342">
         <v>200133</v>
       </c>
       <c r="C342" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="343" spans="1:3">
       <c r="A343" s="1">
-        <v>6699</v>
+        <v>6950</v>
       </c>
       <c r="B343">
-        <v>200133</v>
+        <v>200134</v>
       </c>
       <c r="C343" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="344" spans="1:3">
       <c r="A344" s="1">
-        <v>6938</v>
+        <v>6951</v>
       </c>
       <c r="B344">
-        <v>200133</v>
+        <v>200134</v>
       </c>
       <c r="C344" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="345" spans="1:3">
       <c r="A345" s="1">
-        <v>6950</v>
+        <v>6981</v>
       </c>
       <c r="B345">
-        <v>200134</v>
+        <v>200110</v>
       </c>
       <c r="C345" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="346" spans="1:3">
       <c r="A346" s="1">
-        <v>6951</v>
+        <v>6983</v>
       </c>
       <c r="B346">
-        <v>200134</v>
+        <v>200110</v>
       </c>
       <c r="C346" t="s">
-        <v>309</v>
+        <v>26</v>
       </c>
     </row>
     <row r="347" spans="1:3">
       <c r="A347" s="1">
-        <v>6981</v>
+        <v>6984</v>
       </c>
       <c r="B347">
         <v>200110</v>
       </c>
       <c r="C347" t="s">
-        <v>310</v>
+        <v>2</v>
       </c>
     </row>
     <row r="348" spans="1:3">
       <c r="A348" s="1">
-        <v>6983</v>
+        <v>6985</v>
       </c>
       <c r="B348">
         <v>200110</v>
       </c>
       <c r="C348" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="349" spans="1:3">
-      <c r="A349" s="1">
-        <v>6984</v>
-      </c>
-      <c r="B349">
-        <v>200110</v>
-      </c>
-      <c r="C349" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="350" spans="1:3">
-      <c r="A350" s="1">
-        <v>6985</v>
-      </c>
-      <c r="B350">
-        <v>200110</v>
-      </c>
-      <c r="C350" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First data upload all keyflows
</commit_message>
<xml_diff>
--- a/Public_data/Exports_CG_part1/Export_LMA_compositions.xlsx
+++ b/Public_data/Exports_CG_part1/Export_LMA_compositions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="1657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="1629">
   <si>
     <t>EuralCode</t>
   </si>
@@ -4804,175 +4804,52 @@
     <t>vernietiging knoopcel lithiumbatterijen</t>
   </si>
   <si>
-    <t>puin met max. 70 % grond</t>
-  </si>
-  <si>
-    <t>puin met &gt; 30% zand</t>
-  </si>
-  <si>
-    <t>grond en stenen</t>
-  </si>
-  <si>
-    <t>grond en stenen &gt; 20 %</t>
-  </si>
-  <si>
-    <t>steenkorrel/puingranulaat 0/31</t>
-  </si>
-  <si>
-    <t>zand bkk tot indicatief indust</t>
-  </si>
-  <si>
-    <t>bovengrond klasse wonen - bkk</t>
-  </si>
-  <si>
-    <t>zeefgrond met wortels en overi</t>
-  </si>
-  <si>
-    <t>grond/zand land/natuur &lt; 100 m</t>
-  </si>
-  <si>
-    <t>porselein</t>
-  </si>
-  <si>
-    <t>porcelein</t>
-  </si>
-  <si>
-    <t>medicijnen</t>
-  </si>
-  <si>
-    <t>gemengd- en containerpuin &lt; 70</t>
-  </si>
-  <si>
-    <t>6347 grond &lt; 10 ton zonder ver</t>
-  </si>
-  <si>
-    <t>3240 puin gemengd &lt; 70 cm</t>
-  </si>
-  <si>
-    <t>6348 grond &gt; 10 ton zonder ver</t>
-  </si>
-  <si>
-    <t>licht verontreinigde grond</t>
-  </si>
-  <si>
-    <t>bbk aw zand ingaand</t>
-  </si>
-  <si>
-    <t>ongekeurd / onverdacht grond</t>
-  </si>
-  <si>
-    <t>licht verontreinigde grond ingaand</t>
-  </si>
-  <si>
-    <t>schone grond</t>
-  </si>
-  <si>
-    <t>puin uit grond</t>
-  </si>
-  <si>
-    <t>gft stenen</t>
-  </si>
-  <si>
-    <t>gemengd- en containerpuin &amp;amp;lt; 70 cm</t>
-  </si>
-  <si>
-    <t>6404 zand/grond klasse wonen</t>
-  </si>
-  <si>
-    <t>grond en stenen (tuin- en plantsoenafval (inclusief afval van begr</t>
-  </si>
-  <si>
-    <t>verwachte woongrond</t>
-  </si>
-  <si>
-    <t>aw vrijtoepasbare grond</t>
-  </si>
-  <si>
-    <t>verwachte industriegrond puin</t>
-  </si>
-  <si>
-    <t>grond vrij van stenen/ puin</t>
-  </si>
-  <si>
-    <t>ongekeurde grond</t>
-  </si>
-  <si>
-    <t>6347 grond &lt; 10 ton zonder verklaring</t>
-  </si>
-  <si>
-    <t>6348 grond &gt; 10 ton zonder verklaring</t>
-  </si>
-  <si>
-    <t>240 puin &amp;amp;lt; 70 cm schoon</t>
-  </si>
-  <si>
-    <t>6348 grond &gt;10 ton zonder verk</t>
-  </si>
-  <si>
-    <t>6347 grond &lt; ton zonder verkla</t>
-  </si>
-  <si>
-    <t>niet onder 170503 vallende steen en grond</t>
-  </si>
-  <si>
-    <t>grond, dnacc penningweg 38, 1827 jm alkmaar</t>
-  </si>
-  <si>
-    <t>grond, dnacc ,kruidenierspeerstraat 5, zuid oost beemster</t>
-  </si>
-  <si>
-    <t>grond, dnacc han hoekstrahof 136</t>
-  </si>
-  <si>
-    <t>grond, andijk</t>
-  </si>
-  <si>
-    <t>grond, dnacc, venneweg 2, berkhout</t>
-  </si>
-  <si>
-    <t>grond, dnacc, middenweg 32, bovenkarspel</t>
-  </si>
-  <si>
-    <t>grond, dnacc tuinstraat 23, medemblik</t>
-  </si>
-  <si>
-    <t>grond, dnacc, eerste groenlaan 125, castricum</t>
-  </si>
-  <si>
-    <t>grond, dnacc, pr willem alexandersingel 45, den helder</t>
-  </si>
-  <si>
-    <t>grond, paltrokmolen 8, noord-scharwoude</t>
-  </si>
-  <si>
-    <t>grond, veenrug 68, wognum</t>
-  </si>
-  <si>
-    <t>grond, dnacc, hoge weere 83, zwaag</t>
-  </si>
-  <si>
-    <t>grond, van gelder, pieter zeemanweg 1, zuid-scharwoude</t>
-  </si>
-  <si>
-    <t>grond, kennemerstraatweg 580, heiloo</t>
-  </si>
-  <si>
-    <t>dnacc, hhw, weidemolen 4 i</t>
-  </si>
-  <si>
-    <t>zand/grond/klei gestort (klasse industrie)</t>
-  </si>
-  <si>
-    <t>schone grond, niet route</t>
-  </si>
-  <si>
-    <t>grond (schoon)</t>
-  </si>
-  <si>
-    <t>grond schoon</t>
-  </si>
-  <si>
-    <t>riwi</t>
+    <t>koelkasten en diepvriezers</t>
+  </si>
+  <si>
+    <t>afgedankte apparatuur die chloorfluorkoolstoffen bevat</t>
+  </si>
+  <si>
+    <t>afgedankte apparatuur die chloorfluorkoolwaterstoffen bevat</t>
+  </si>
+  <si>
+    <t>koelkasten per stuk, niet route</t>
+  </si>
+  <si>
+    <t>koelkasten, -apparatuur professioneel</t>
+  </si>
+  <si>
+    <t>1120 koel- en vries apparatuur</t>
+  </si>
+  <si>
+    <t>koelingen</t>
+  </si>
+  <si>
+    <t>koel en vries app</t>
+  </si>
+  <si>
+    <t>koel en vries apparatuur</t>
+  </si>
+  <si>
+    <t>koel en vries app, waterkoelers</t>
+  </si>
+  <si>
+    <t>koel en vries apparaten</t>
+  </si>
+  <si>
+    <t>radarsnelheidapparatuur</t>
+  </si>
+  <si>
+    <t>inbouwapparatuur radarvoertuigen</t>
+  </si>
+  <si>
+    <t>koel en vrieskisten</t>
+  </si>
+  <si>
+    <t>koelkasten/diepvriezers/koelinstallatie</t>
+  </si>
+  <si>
+    <t>airco unit(s)</t>
   </si>
   <si>
     <t>niet onder 20 01 33 vallende batterijen en accus</t>
@@ -4985,6 +4862,45 @@
   </si>
   <si>
     <t>textiel, ter vernietiging</t>
+  </si>
+  <si>
+    <t>afval van bewerking en afwerking</t>
+  </si>
+  <si>
+    <t>melamine-ureum/formaline co polymeer</t>
+  </si>
+  <si>
+    <t>afval van composietmaterialen (ge?mpregneerde textiel, elastomeren, plastomeren)</t>
+  </si>
+  <si>
+    <t>afval van composietmaterialen (geimpregneerde textiel, elastomeren, plastomeren)</t>
+  </si>
+  <si>
+    <t>linoleum met pvc</t>
+  </si>
+  <si>
+    <t>slib van productie van polyprop</t>
+  </si>
+  <si>
+    <t>industrieel slib (ba)</t>
+  </si>
+  <si>
+    <t>zuiveringslib van tapijtindustrie</t>
+  </si>
+  <si>
+    <t>slib</t>
+  </si>
+  <si>
+    <t>loogafval</t>
+  </si>
+  <si>
+    <t>kleurstoffen en pigmenten die gevaarlijke stoffen bevatten</t>
+  </si>
+  <si>
+    <t>slib van afvalwaterbehandeling ter plaatse dat gevaarlijke stoffen bevat</t>
+  </si>
+  <si>
+    <t>afval van afwerking dat organische oplosmiddelen bevat</t>
   </si>
 </sst>
 </file>
@@ -5342,7 +5258,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1752"/>
+  <dimension ref="A1:C1733"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -23907,7 +23823,7 @@
         <v>48708</v>
       </c>
       <c r="B1688">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1688" t="s">
         <v>1596</v>
@@ -23915,10 +23831,10 @@
     </row>
     <row r="1689" spans="1:3">
       <c r="A1689" s="1">
-        <v>48709</v>
+        <v>48711</v>
       </c>
       <c r="B1689">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1689" t="s">
         <v>1597</v>
@@ -23926,10 +23842,10 @@
     </row>
     <row r="1690" spans="1:3">
       <c r="A1690" s="1">
-        <v>48710</v>
+        <v>48714</v>
       </c>
       <c r="B1690">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1690" t="s">
         <v>1598</v>
@@ -23940,681 +23856,472 @@
         <v>48722</v>
       </c>
       <c r="B1691">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1691" t="s">
-        <v>1599</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1692" spans="1:3">
       <c r="A1692" s="1">
-        <v>48723</v>
+        <v>48737</v>
       </c>
       <c r="B1692">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1692" t="s">
-        <v>1600</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1693" spans="1:3">
       <c r="A1693" s="1">
-        <v>48724</v>
+        <v>48756</v>
       </c>
       <c r="B1693">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1693" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="1694" spans="1:3">
       <c r="A1694" s="1">
-        <v>48725</v>
+        <v>48761</v>
       </c>
       <c r="B1694">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1694" t="s">
-        <v>1602</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="1695" spans="1:3">
       <c r="A1695" s="1">
-        <v>48744</v>
+        <v>48762</v>
       </c>
       <c r="B1695">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1695" t="s">
-        <v>1603</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="1696" spans="1:3">
       <c r="A1696" s="1">
-        <v>48754</v>
+        <v>48771</v>
       </c>
       <c r="B1696">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1696" t="s">
-        <v>1604</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1697" spans="1:3">
       <c r="A1697" s="1">
-        <v>48757</v>
+        <v>48779</v>
       </c>
       <c r="B1697">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1697" t="s">
-        <v>1605</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="1698" spans="1:3">
       <c r="A1698" s="1">
-        <v>48767</v>
+        <v>48817</v>
       </c>
       <c r="B1698">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1698" t="s">
-        <v>1606</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="1699" spans="1:3">
       <c r="A1699" s="1">
-        <v>48772</v>
+        <v>48834</v>
       </c>
       <c r="B1699">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1699" t="s">
-        <v>1607</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="1700" spans="1:3">
       <c r="A1700" s="1">
-        <v>48779</v>
+        <v>48853</v>
       </c>
       <c r="B1700">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1700" t="s">
-        <v>361</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="1701" spans="1:3">
       <c r="A1701" s="1">
-        <v>48794</v>
+        <v>48931</v>
       </c>
       <c r="B1701">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1701" t="s">
-        <v>1608</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="1702" spans="1:3">
       <c r="A1702" s="1">
-        <v>48796</v>
+        <v>48939</v>
       </c>
       <c r="B1702">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1702" t="s">
-        <v>1609</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="1703" spans="1:3">
       <c r="A1703" s="1">
-        <v>48797</v>
+        <v>48952</v>
       </c>
       <c r="B1703">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1703" t="s">
-        <v>1610</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="1704" spans="1:3">
       <c r="A1704" s="1">
-        <v>48799</v>
+        <v>48961</v>
       </c>
       <c r="B1704">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1704" t="s">
-        <v>1611</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="1705" spans="1:3">
       <c r="A1705" s="1">
-        <v>48805</v>
+        <v>48977</v>
       </c>
       <c r="B1705">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1705" t="s">
-        <v>1612</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="1706" spans="1:3">
       <c r="A1706" s="1">
-        <v>48807</v>
+        <v>48980</v>
       </c>
       <c r="B1706">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1706" t="s">
-        <v>1613</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="1707" spans="1:3">
       <c r="A1707" s="1">
-        <v>48808</v>
+        <v>48999</v>
       </c>
       <c r="B1707">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1707" t="s">
-        <v>1614</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="1708" spans="1:3">
       <c r="A1708" s="1">
-        <v>48809</v>
+        <v>49000</v>
       </c>
       <c r="B1708">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1708" t="s">
-        <v>1615</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="1709" spans="1:3">
       <c r="A1709" s="1">
-        <v>48816</v>
+        <v>49004</v>
       </c>
       <c r="B1709">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1709" t="s">
-        <v>1616</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="1710" spans="1:3">
       <c r="A1710" s="1">
-        <v>48822</v>
+        <v>49035</v>
       </c>
       <c r="B1710">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1710" t="s">
-        <v>1617</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="1711" spans="1:3">
       <c r="A1711" s="1">
-        <v>48824</v>
+        <v>49037</v>
       </c>
       <c r="B1711">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1711" t="s">
-        <v>1618</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="1712" spans="1:3">
       <c r="A1712" s="1">
-        <v>48850</v>
+        <v>49041</v>
       </c>
       <c r="B1712">
-        <v>200202</v>
+        <v>200123</v>
       </c>
       <c r="C1712" t="s">
-        <v>1619</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1713" spans="1:3">
       <c r="A1713" s="1">
-        <v>48882</v>
+        <v>49154</v>
       </c>
       <c r="B1713">
-        <v>200202</v>
+        <v>200134</v>
       </c>
       <c r="C1713" t="s">
-        <v>1620</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="1714" spans="1:3">
       <c r="A1714" s="1">
-        <v>48896</v>
+        <v>49155</v>
       </c>
       <c r="B1714">
-        <v>200202</v>
+        <v>200134</v>
       </c>
       <c r="C1714" t="s">
-        <v>1621</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="1715" spans="1:3">
       <c r="A1715" s="1">
-        <v>48901</v>
+        <v>49185</v>
       </c>
       <c r="B1715">
-        <v>200202</v>
+        <v>200110</v>
       </c>
       <c r="C1715" t="s">
-        <v>1622</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="1716" spans="1:3">
       <c r="A1716" s="1">
-        <v>48903</v>
+        <v>49187</v>
       </c>
       <c r="B1716">
-        <v>200202</v>
+        <v>200110</v>
       </c>
       <c r="C1716" t="s">
-        <v>1623</v>
+        <v>185</v>
       </c>
     </row>
     <row r="1717" spans="1:3">
       <c r="A1717" s="1">
-        <v>48904</v>
+        <v>49188</v>
       </c>
       <c r="B1717">
-        <v>200202</v>
+        <v>200110</v>
       </c>
       <c r="C1717" t="s">
-        <v>1624</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="1718" spans="1:3">
       <c r="A1718" s="1">
-        <v>48908</v>
+        <v>49189</v>
       </c>
       <c r="B1718">
-        <v>200202</v>
+        <v>200110</v>
       </c>
       <c r="C1718" t="s">
-        <v>1625</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="1719" spans="1:3">
       <c r="A1719" s="1">
-        <v>48910</v>
+        <v>49190</v>
       </c>
       <c r="B1719">
-        <v>200202</v>
+        <v>40109</v>
       </c>
       <c r="C1719" t="s">
-        <v>294</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="1720" spans="1:3">
       <c r="A1720" s="1">
-        <v>48913</v>
+        <v>49191</v>
       </c>
       <c r="B1720">
-        <v>200202</v>
+        <v>40109</v>
       </c>
       <c r="C1720" t="s">
-        <v>1626</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="1721" spans="1:3">
       <c r="A1721" s="1">
-        <v>48914</v>
+        <v>49192</v>
       </c>
       <c r="B1721">
-        <v>200202</v>
+        <v>40222</v>
       </c>
       <c r="C1721" t="s">
-        <v>1627</v>
+        <v>753</v>
       </c>
     </row>
     <row r="1722" spans="1:3">
       <c r="A1722" s="1">
-        <v>48916</v>
+        <v>49193</v>
       </c>
       <c r="B1722">
-        <v>200202</v>
+        <v>40209</v>
       </c>
       <c r="C1722" t="s">
-        <v>1628</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="1723" spans="1:3">
       <c r="A1723" s="1">
-        <v>48917</v>
+        <v>49198</v>
       </c>
       <c r="B1723">
-        <v>200202</v>
+        <v>40209</v>
       </c>
       <c r="C1723" t="s">
-        <v>1629</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="1724" spans="1:3">
       <c r="A1724" s="1">
-        <v>48936</v>
+        <v>49199</v>
       </c>
       <c r="B1724">
-        <v>200202</v>
+        <v>40209</v>
       </c>
       <c r="C1724" t="s">
-        <v>1630</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="1725" spans="1:3">
       <c r="A1725" s="1">
-        <v>48953</v>
+        <v>49200</v>
       </c>
       <c r="B1725">
-        <v>200202</v>
+        <v>40220</v>
       </c>
       <c r="C1725" t="s">
-        <v>1631</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="1726" spans="1:3">
       <c r="A1726" s="1">
-        <v>48972</v>
+        <v>49206</v>
       </c>
       <c r="B1726">
-        <v>200202</v>
+        <v>40220</v>
       </c>
       <c r="C1726" t="s">
-        <v>1632</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="1727" spans="1:3">
       <c r="A1727" s="1">
-        <v>49024</v>
+        <v>49219</v>
       </c>
       <c r="B1727">
-        <v>200202</v>
+        <v>40220</v>
       </c>
       <c r="C1727" t="s">
-        <v>1633</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="1728" spans="1:3">
       <c r="A1728" s="1">
-        <v>49025</v>
+        <v>49229</v>
       </c>
       <c r="B1728">
-        <v>200202</v>
+        <v>40220</v>
       </c>
       <c r="C1728" t="s">
-        <v>1634</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="1729" spans="1:3">
       <c r="A1729" s="1">
-        <v>49026</v>
+        <v>49230</v>
       </c>
       <c r="B1729">
-        <v>200202</v>
+        <v>40106</v>
       </c>
       <c r="C1729" t="s">
-        <v>1635</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="1730" spans="1:3">
       <c r="A1730" s="1">
-        <v>49027</v>
+        <v>49231</v>
       </c>
       <c r="B1730">
-        <v>200202</v>
+        <v>40102</v>
       </c>
       <c r="C1730" t="s">
-        <v>1636</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="1731" spans="1:3">
       <c r="A1731" s="1">
-        <v>49029</v>
+        <v>49235</v>
       </c>
       <c r="B1731">
-        <v>200202</v>
+        <v>40216</v>
       </c>
       <c r="C1731" t="s">
-        <v>1637</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="1732" spans="1:3">
       <c r="A1732" s="1">
-        <v>49030</v>
+        <v>49257</v>
       </c>
       <c r="B1732">
-        <v>200202</v>
+        <v>40219</v>
       </c>
       <c r="C1732" t="s">
-        <v>1638</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="1733" spans="1:3">
       <c r="A1733" s="1">
-        <v>49031</v>
+        <v>49260</v>
       </c>
       <c r="B1733">
-        <v>200202</v>
+        <v>40214</v>
       </c>
       <c r="C1733" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="1734" spans="1:3">
-      <c r="A1734" s="1">
-        <v>49032</v>
-      </c>
-      <c r="B1734">
-        <v>200202</v>
-      </c>
-      <c r="C1734" t="s">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="1735" spans="1:3">
-      <c r="A1735" s="1">
-        <v>49033</v>
-      </c>
-      <c r="B1735">
-        <v>200202</v>
-      </c>
-      <c r="C1735" t="s">
-        <v>1641</v>
-      </c>
-    </row>
-    <row r="1736" spans="1:3">
-      <c r="A1736" s="1">
-        <v>49034</v>
-      </c>
-      <c r="B1736">
-        <v>200202</v>
-      </c>
-      <c r="C1736" t="s">
-        <v>1642</v>
-      </c>
-    </row>
-    <row r="1737" spans="1:3">
-      <c r="A1737" s="1">
-        <v>49035</v>
-      </c>
-      <c r="B1737">
-        <v>200202</v>
-      </c>
-      <c r="C1737" t="s">
-        <v>1643</v>
-      </c>
-    </row>
-    <row r="1738" spans="1:3">
-      <c r="A1738" s="1">
-        <v>49036</v>
-      </c>
-      <c r="B1738">
-        <v>200202</v>
-      </c>
-      <c r="C1738" t="s">
-        <v>1644</v>
-      </c>
-    </row>
-    <row r="1739" spans="1:3">
-      <c r="A1739" s="1">
-        <v>49037</v>
-      </c>
-      <c r="B1739">
-        <v>200202</v>
-      </c>
-      <c r="C1739" t="s">
-        <v>1645</v>
-      </c>
-    </row>
-    <row r="1740" spans="1:3">
-      <c r="A1740" s="1">
-        <v>49038</v>
-      </c>
-      <c r="B1740">
-        <v>200202</v>
-      </c>
-      <c r="C1740" t="s">
-        <v>1646</v>
-      </c>
-    </row>
-    <row r="1741" spans="1:3">
-      <c r="A1741" s="1">
-        <v>49039</v>
-      </c>
-      <c r="B1741">
-        <v>200202</v>
-      </c>
-      <c r="C1741" t="s">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="1742" spans="1:3">
-      <c r="A1742" s="1">
-        <v>49042</v>
-      </c>
-      <c r="B1742">
-        <v>200202</v>
-      </c>
-      <c r="C1742" t="s">
-        <v>1648</v>
-      </c>
-    </row>
-    <row r="1743" spans="1:3">
-      <c r="A1743" s="1">
-        <v>49044</v>
-      </c>
-      <c r="B1743">
-        <v>200202</v>
-      </c>
-      <c r="C1743" t="s">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="1744" spans="1:3">
-      <c r="A1744" s="1">
-        <v>49045</v>
-      </c>
-      <c r="B1744">
-        <v>200202</v>
-      </c>
-      <c r="C1744" t="s">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="1745" spans="1:3">
-      <c r="A1745" s="1">
-        <v>49047</v>
-      </c>
-      <c r="B1745">
-        <v>200202</v>
-      </c>
-      <c r="C1745" t="s">
-        <v>1651</v>
-      </c>
-    </row>
-    <row r="1746" spans="1:3">
-      <c r="A1746" s="1">
-        <v>49050</v>
-      </c>
-      <c r="B1746">
-        <v>200202</v>
-      </c>
-      <c r="C1746" t="s">
-        <v>1652</v>
-      </c>
-    </row>
-    <row r="1747" spans="1:3">
-      <c r="A1747" s="1">
-        <v>49051</v>
-      </c>
-      <c r="B1747">
-        <v>200134</v>
-      </c>
-      <c r="C1747" t="s">
-        <v>1653</v>
-      </c>
-    </row>
-    <row r="1748" spans="1:3">
-      <c r="A1748" s="1">
-        <v>49052</v>
-      </c>
-      <c r="B1748">
-        <v>200134</v>
-      </c>
-      <c r="C1748" t="s">
-        <v>1654</v>
-      </c>
-    </row>
-    <row r="1749" spans="1:3">
-      <c r="A1749" s="1">
-        <v>49082</v>
-      </c>
-      <c r="B1749">
-        <v>200110</v>
-      </c>
-      <c r="C1749" t="s">
-        <v>1655</v>
-      </c>
-    </row>
-    <row r="1750" spans="1:3">
-      <c r="A1750" s="1">
-        <v>49084</v>
-      </c>
-      <c r="B1750">
-        <v>200110</v>
-      </c>
-      <c r="C1750" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="1751" spans="1:3">
-      <c r="A1751" s="1">
-        <v>49085</v>
-      </c>
-      <c r="B1751">
-        <v>200110</v>
-      </c>
-      <c r="C1751" t="s">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="1752" spans="1:3">
-      <c r="A1752" s="1">
-        <v>49086</v>
-      </c>
-      <c r="B1752">
-        <v>200110</v>
-      </c>
-      <c r="C1752" t="s">
-        <v>1656</v>
+        <v>1628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>